<commit_message>
adding 501c type classification
</commit_message>
<xml_diff>
--- a/tax-exempt-status/data-raw/subsection-classification.xlsx
+++ b/tax-exempt-status/data-raw/subsection-classification.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviabeck/Box Sync/metadata-standards/tax-exempt-status/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E886EAD-F68F-2A4F-A364-108B45DB562B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DA2CED-7255-F74B-8A86-98E37AA7017C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15760" xr2:uid="{CD049C6F-8F82-314F-A9EE-194A03592E85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -219,7 +219,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +231,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="ArialMT"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -250,14 +258,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -572,9 +583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D67A78-180F-8C48-B8E5-4242B1403812}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C34" sqref="C34"/>
+      <selection pane="topRight" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -973,11 +984,14 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A42" r:id="rId1" xr:uid="{99216050-EE1D-AB4E-B98A-0F4BA5CDF7EC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>